<commit_message>
Sửa lại cây thư mục theo phân công, viết code theo phân công
Sửa lại cây thư mục theo phân công, viết code theo phân công
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan9.xlsx
+++ b/plan/kehoachphancong_tuan9.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\thanhsang\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE47F99-8E27-4146-8660-F2B84B815A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46BC59A-CEF8-4306-A096-A712607A0179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,33 +495,6 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -547,6 +520,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -877,445 +877,449 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
+      <c r="C9" s="28"/>
+      <c r="D9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="28"/>
+      <c r="F9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="16" t="s">
+      <c r="G9" s="30"/>
+      <c r="H9" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="17" t="s">
+      <c r="I9" s="28"/>
+      <c r="J9" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="16" t="s">
+      <c r="K9" s="30"/>
+      <c r="L9" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="16" t="s">
+      <c r="M9" s="28"/>
+      <c r="N9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="17"/>
+      <c r="O9" s="30"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20" t="s">
+      <c r="C10" s="25"/>
+      <c r="D10" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="21" t="s">
+      <c r="E10" s="25"/>
+      <c r="F10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="20" t="s">
+      <c r="G10" s="23"/>
+      <c r="H10" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="21" t="s">
+      <c r="I10" s="25"/>
+      <c r="J10" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="21"/>
-      <c r="L10" s="20" t="s">
+      <c r="K10" s="23"/>
+      <c r="L10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="20" t="s">
+      <c r="M10" s="25"/>
+      <c r="N10" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="O10" s="21"/>
+      <c r="O10" s="23"/>
     </row>
     <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K11" s="24" t="s">
+      <c r="K11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L11" s="23" t="s">
+      <c r="L11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="M11" s="24" t="s">
+      <c r="M11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="23" t="s">
+      <c r="N11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O11" s="24" t="s">
+      <c r="O11" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="378.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="30"/>
+      <c r="C12" s="21">
+        <v>1</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="21"/>
     </row>
     <row r="13" spans="1:15" ht="309" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="27"/>
+      <c r="C13" s="18">
+        <v>1</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="18"/>
     </row>
     <row r="14" spans="1:15" ht="134.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="30"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="21"/>
     </row>
     <row r="15" spans="1:15" ht="355.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="27"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="18"/>
     </row>
     <row r="16" spans="1:15" ht="387" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="30"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="21"/>
     </row>
     <row r="17" spans="1:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="27"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="18"/>
     </row>
     <row r="18" spans="1:15" ht="79.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="30"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="21"/>
     </row>
     <row r="19" spans="1:15" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="27"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="18"/>
     </row>
     <row r="20" spans="1:15" ht="185.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="30"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="21"/>
     </row>
     <row r="21" spans="1:15" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="27"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="18"/>
     </row>
     <row r="22" spans="1:15" ht="79.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -1473,13 +1477,6 @@
     <row r="31" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -1488,6 +1485,13 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
đánh dấu hoàn thành theo phân công
đánh dấu hoàn thành theo phân công
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan9.xlsx
+++ b/plan/kehoachphancong_tuan9.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E110C73-150A-42B1-89EA-07AC88810D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A8CCC8-A085-44D3-A7EC-B6456A3CF6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,6 +522,18 @@
     <xf numFmtId="164" fontId="10" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -535,18 +547,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -866,7 +866,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -877,204 +877,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="28"/>
+      <c r="D9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="26" t="s">
+      <c r="E9" s="28"/>
+      <c r="F9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="25" t="s">
+      <c r="G9" s="30"/>
+      <c r="H9" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="26" t="s">
+      <c r="I9" s="28"/>
+      <c r="J9" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="25" t="s">
+      <c r="K9" s="30"/>
+      <c r="L9" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="24"/>
-      <c r="N9" s="25" t="s">
+      <c r="M9" s="28"/>
+      <c r="N9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="26"/>
+      <c r="O9" s="30"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="25"/>
+      <c r="D10" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="28" t="s">
+      <c r="E10" s="25"/>
+      <c r="F10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="27" t="s">
+      <c r="G10" s="23"/>
+      <c r="H10" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="28" t="s">
+      <c r="I10" s="25"/>
+      <c r="J10" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="28"/>
-      <c r="L10" s="27" t="s">
+      <c r="K10" s="23"/>
+      <c r="L10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="27" t="s">
+      <c r="M10" s="25"/>
+      <c r="N10" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="O10" s="28"/>
+      <c r="O10" s="23"/>
     </row>
     <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
@@ -1245,7 +1245,9 @@
       <c r="B17" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="18">
+        <v>1</v>
+      </c>
       <c r="D17" s="17"/>
       <c r="E17" s="18"/>
       <c r="F17" s="17"/>
@@ -1483,13 +1485,6 @@
     <row r="31" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -1498,6 +1493,13 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>